<commit_message>
updated gps, random particles, and starting to integrate compass
</commit_message>
<xml_diff>
--- a/competition.xlsx
+++ b/competition.xlsx
@@ -4,7 +4,8 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10230" yWindow="-15" windowWidth="10275" windowHeight="8175"/>
+    <workbookView xWindow="6810" yWindow="0" windowWidth="13515" windowHeight="8160"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="6825" windowHeight="8175" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>x</t>
   </si>
@@ -73,6 +74,9 @@
   </si>
   <si>
     <t>t (*pi)</t>
+  </si>
+  <si>
+    <t>wall following</t>
   </si>
 </sst>
 </file>
@@ -489,10 +493,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>traj!$B$2:$B$215</c:f>
+              <c:f>traj!$B$2:$B$217</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="214"/>
+                <c:ptCount val="216"/>
                 <c:pt idx="0">
                   <c:v>1.5</c:v>
                 </c:pt>
@@ -520,7 +524,19 @@
                 <c:pt idx="16">
                   <c:v>13</c:v>
                 </c:pt>
+                <c:pt idx="18">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>20</c:v>
+                </c:pt>
                 <c:pt idx="24">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
@@ -528,10 +544,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>traj!$C$2:$C$215</c:f>
+              <c:f>traj!$C$2:$C$217</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="214"/>
+                <c:ptCount val="216"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -559,7 +575,19 @@
                 <c:pt idx="16">
                   <c:v>-26</c:v>
                 </c:pt>
+                <c:pt idx="18">
+                  <c:v>-26</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-9</c:v>
+                </c:pt>
                 <c:pt idx="24">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>-27</c:v>
                 </c:pt>
               </c:numCache>
@@ -575,11 +603,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="81733888"/>
-        <c:axId val="42586496"/>
+        <c:axId val="68146304"/>
+        <c:axId val="68148224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81733888"/>
+        <c:axId val="68146304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -591,12 +619,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42586496"/>
+        <c:crossAx val="68148224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42586496"/>
+        <c:axId val="68148224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -608,7 +636,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81733888"/>
+        <c:crossAx val="68146304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -949,9 +977,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
+    <sheetView topLeftCell="A10" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2024,13 +2053,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="1">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2040,8 +2072,11 @@
       <c r="D1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -2055,7 +2090,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1.5</v>
       </c>
@@ -2066,7 +2101,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1.5</v>
       </c>
@@ -2077,7 +2112,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2091,7 +2126,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>0</v>
       </c>
@@ -2102,7 +2137,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>1</v>
       </c>
@@ -2113,7 +2148,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>4</v>
       </c>
@@ -2124,7 +2159,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>8</v>
       </c>
@@ -2135,7 +2170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>13</v>
       </c>
@@ -2146,14 +2181,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>16</v>
-      </c>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>-26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>-21</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>20</v>
+      </c>
+      <c r="C24">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>50</v>
       </c>
       <c r="C26">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28">
+        <v>50</v>
+      </c>
+      <c r="C28">
         <v>-27</v>
       </c>
     </row>
@@ -2167,6 +2237,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
updated map and wall tracking
</commit_message>
<xml_diff>
--- a/competition.xlsx
+++ b/competition.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="6810" yWindow="0" windowWidth="13515" windowHeight="8160"/>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="6825" windowHeight="8175" activeTab="1"/>
+    <workbookView xWindow="6825" yWindow="-15" windowWidth="13515" windowHeight="8160"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="6825" windowHeight="8175" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
     <sheet name="traj" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="traj2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>x</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>wall following</t>
+  </si>
+  <si>
+    <t>rotate</t>
   </si>
 </sst>
 </file>
@@ -163,10 +166,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>map!$B$3:$B$61</c:f>
+              <c:f>map!$B$3:$B$200</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="198"/>
                 <c:pt idx="0">
                   <c:v>1.8305</c:v>
                 </c:pt>
@@ -315,6 +318,9 @@
                   <c:v>21.655499999999996</c:v>
                 </c:pt>
                 <c:pt idx="58">
+                  <c:v>56.847499999999997</c:v>
+                </c:pt>
+                <c:pt idx="59">
                   <c:v>56.847499999999997</c:v>
                 </c:pt>
               </c:numCache>
@@ -322,10 +328,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>map!$C$3:$C$61</c:f>
+              <c:f>map!$C$3:$C$200</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="198"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -475,6 +481,9 @@
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>-10.600499999999995</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-6.87</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -595,6 +604,116 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>traj2</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>traj2!$B$2:$B$200</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="199"/>
+                <c:pt idx="0">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>traj2!$C$2:$C$200</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="199"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-19</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-21</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-26</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-26</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-26</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-26</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-26</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-27</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -603,11 +722,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="68146304"/>
-        <c:axId val="68148224"/>
+        <c:axId val="67165184"/>
+        <c:axId val="83197312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="68146304"/>
+        <c:axId val="67165184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -619,12 +738,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68148224"/>
+        <c:crossAx val="83197312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68148224"/>
+        <c:axId val="83197312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -636,7 +755,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68146304"/>
+        <c:crossAx val="67165184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -975,12 +1094,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
-    <sheetView topLeftCell="A10" workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2043,6 +2164,14 @@
       <c r="G61">
         <f>G54</f>
         <v>17.677499999999995</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>56.847499999999997</v>
+      </c>
+      <c r="C62">
+        <v>-6.87</v>
       </c>
     </row>
   </sheetData>
@@ -2055,9 +2184,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="1">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A2" workbookViewId="0"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="E6" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2188,6 +2317,9 @@
       <c r="C20">
         <v>-26</v>
       </c>
+      <c r="D20">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22">
@@ -2234,13 +2366,187 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView topLeftCell="A2" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>1.5</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1.5</v>
+      </c>
+      <c r="C4">
+        <v>-8.6999999999999993</v>
+      </c>
+      <c r="D4">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1.5</v>
+      </c>
+      <c r="C6">
+        <v>-14</v>
+      </c>
+      <c r="D6">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>-19</v>
+      </c>
+      <c r="D8">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>-21</v>
+      </c>
+      <c r="D10">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>-26</v>
+      </c>
+      <c r="D12">
+        <v>-0.5</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>-26</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>-26</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>-26</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>-26</v>
+      </c>
+      <c r="D20">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>-21</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>20</v>
+      </c>
+      <c r="C24">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>50</v>
+      </c>
+      <c r="C26">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28">
+        <v>50</v>
+      </c>
+      <c r="C28">
+        <v>-27</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>